<commit_message>
Gain resistors updated to 1k, 100
</commit_message>
<xml_diff>
--- a/fmcboard_eagle/BOM_JLCSMT.xlsx
+++ b/fmcboard_eagle/BOM_JLCSMT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitwork\LL10G_Cyclone10GX_1\fmcboard_eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960156B9-7239-4020-9A5C-A4FEB259EE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F17DEB-7882-4361-9674-EA5FF506A175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39765" yWindow="1725" windowWidth="31035" windowHeight="15915" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
   <si>
     <t>Comment</t>
   </si>
@@ -128,9 +128,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R1, R6, R7, R8, R9, R12, R13, R18, R20, R21, R22, R23, R24, R27, R28, R29, R30, R32, R33, R36, R38, R40</t>
-  </si>
-  <si>
     <t>1pF</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>SV1, SV2</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>R10, R19, R26</t>
   </si>
   <si>
@@ -206,12 +200,6 @@
     <t>R42</t>
   </si>
   <si>
-    <t>5k</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>7805TV</t>
   </si>
   <si>
@@ -303,6 +291,9 @@
   </si>
   <si>
     <t>8-pin</t>
+  </si>
+  <si>
+    <t>R1, R6, R7, R8, R9, R11, R12, R13, R18, R20, R21, R22, R23, R24, R27, R28, R29, R30, R32, R33, R36, R38, R40</t>
   </si>
 </sst>
 </file>
@@ -421,14 +412,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -802,329 +793,318 @@
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="8">
+        <v>100</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="7" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="6" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="6" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="6" t="s">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="7" t="s">
+      <c r="B17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="6" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
         <v>46</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
         <v>56</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="7" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
         <v>62</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="7" t="s">
+    </row>
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
         <v>68</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="7" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
         <v>74</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>